<commit_message>
Fixed column names in flexfile enum
</commit_message>
<xml_diff>
--- a/data-raw/flexfile-enumerations.xlsx
+++ b/data-raw/flexfile-enumerations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mstephenson\Software\Git Local\readflexfile\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajames\Software\Git Local\costverse\readflexfile\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="phaseormilestoneenum" sheetId="1" r:id="rId1"/>
@@ -32,13 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="180">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="178">
   <si>
     <t>PRE_A</t>
   </si>
@@ -895,70 +889,70 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -974,174 +968,174 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1157,38 +1151,38 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>56</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1204,38 +1198,38 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1251,30 +1245,30 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>66</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1290,126 +1284,126 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>72</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>74</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>75</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>76</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>77</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>78</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>79</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>80</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>81</v>
       </c>
-      <c r="B13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B15" t="s">
         <v>82</v>
-      </c>
-      <c r="B14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1421,226 +1415,226 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>98</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>99</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>100</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>77</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>103</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>104</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>79</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>108</v>
-      </c>
-      <c r="B21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>109</v>
-      </c>
-      <c r="B22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>110</v>
-      </c>
-      <c r="B23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>81</v>
       </c>
-      <c r="B25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B27" t="s">
         <v>82</v>
-      </c>
-      <c r="B26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1656,30 +1650,30 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>126</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1691,218 +1685,218 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>130</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>131</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>132</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>133</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>134</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>135</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>136</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>137</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>138</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>139</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>140</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>141</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>142</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>143</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>144</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>145</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>146</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>147</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>148</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>149</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>150</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>151</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>152</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>153</v>
-      </c>
-      <c r="B25" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>154</v>
-      </c>
-      <c r="B26" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed case of FlexFile to native
</commit_message>
<xml_diff>
--- a/data-raw/flexfile-enumerations.xlsx
+++ b/data-raw/flexfile-enumerations.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajames\Software\Git Local\costverse\readflexfile\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496D6258-940B-452A-8FA2-CDD4F88FD252}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="phaseormilestoneenum" sheetId="1" r:id="rId1"/>
-    <sheet name="contracttypeenum" sheetId="2" r:id="rId2"/>
-    <sheet name="appropriationtypeenum" sheetId="3" r:id="rId3"/>
+    <sheet name="PhaseOrMilestoneEnum" sheetId="1" r:id="rId1"/>
+    <sheet name="ContractTypeEnum" sheetId="2" r:id="rId2"/>
+    <sheet name="AppropriationTypeEnum" sheetId="3" r:id="rId3"/>
     <sheet name="reportcycleenum" sheetId="4" r:id="rId4"/>
-    <sheet name="nonrecurringorrecurringenum" sheetId="5" r:id="rId5"/>
-    <sheet name="standardcategoryenum" sheetId="6" r:id="rId6"/>
-    <sheet name="detailedstandardcategoryenum" sheetId="7" r:id="rId7"/>
-    <sheet name="allocationmethodtypeenum" sheetId="8" r:id="rId8"/>
-    <sheet name="costhourtagenum" sheetId="9" r:id="rId9"/>
+    <sheet name="NonrecurringOrRecurringEnum" sheetId="5" r:id="rId5"/>
+    <sheet name="StandardCategoryEnum" sheetId="6" r:id="rId6"/>
+    <sheet name="DetailedStandardCategoryEnum" sheetId="7" r:id="rId7"/>
+    <sheet name="AllocationMethodTypeEnum" sheetId="8" r:id="rId8"/>
+    <sheet name="CostHourTagEnum" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -70,12 +71,6 @@
     <t>Multiple</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>CS</t>
   </si>
   <si>
@@ -566,12 +561,18 @@
   </si>
   <si>
     <t>Tag 25</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -882,76 +883,257 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B21" t="s">
         <v>11</v>
       </c>
     </row>
@@ -960,182 +1142,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1143,46 +1189,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1190,46 +1236,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1237,38 +1275,134 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1276,134 +1410,230 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1411,230 +1641,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>104</v>
-      </c>
-      <c r="B19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>107</v>
-      </c>
-      <c r="B22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>108</v>
-      </c>
-      <c r="B23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>109</v>
-      </c>
-      <c r="B24" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1642,261 +1680,222 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>